<commit_message>
Castle of the Dragon - final boss 63 frames faster
</commit_message>
<xml_diff>
--- a/CastleOfTheDragon/Castle.xlsx
+++ b/CastleOfTheDragon/Castle.xlsx
@@ -3277,14 +3277,14 @@
         <v>188</v>
       </c>
       <c r="C50" s="101">
-        <v>23409</v>
+        <v>23345</v>
       </c>
       <c r="D50" s="101">
         <v>25183</v>
       </c>
       <c r="E50" s="123">
         <f t="shared" si="1"/>
-        <v>1774</v>
+        <v>1838</v>
       </c>
       <c r="F50" s="105"/>
     </row>

</xml_diff>